<commit_message>
Added cleanup code to combine columns
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexm\Documents\code\bdcw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{234C86AA-AD78-4D69-B971-69EC2D4DC319}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BC2F1A84-5EC4-443E-ABE2-874AD8A16A0D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="11" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="veil-type" sheetId="21" r:id="rId1"/>
@@ -34,13 +34,15 @@
     <sheet name="cap-color" sheetId="3" r:id="rId19"/>
     <sheet name="population" sheetId="2" r:id="rId20"/>
     <sheet name="bruises" sheetId="1" r:id="rId21"/>
+    <sheet name="prediction" sheetId="22" r:id="rId22"/>
+    <sheet name="Sheet2" sheetId="23" r:id="rId23"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -241,6 +243,12 @@
   </si>
   <si>
     <t>Partial</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>Incorrect</t>
   </si>
 </sst>
 </file>
@@ -724,8 +732,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -8475,6 +8486,584 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>redictions</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>prediction!$A$1:$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Correct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Incorrect</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>prediction!$B$1:$B$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1428</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0B7F-443E-97AC-D9CB0F95811D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="402528024"/>
+        <c:axId val="402519168"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="402528024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="402519168"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="402519168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="402528024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Testing Class</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$1:$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Edible</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Poisonous</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$B$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>709</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>719</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9BA3-4C62-89B0-63C0CF889B12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="229385120"/>
+        <c:axId val="229386432"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="229385120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="229386432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="229386432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="229385120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -12964,6 +13553,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors23.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors24.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -20304,6 +20973,1012 @@
 </file>
 
 <file path=xl/charts/style22.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style23.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style24.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -24965,6 +26640,88 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B71A317-99F1-4EB6-BEFA-D242085A1CED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing23.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47830C95-39CE-4311-AE73-14899F93DEE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -25811,7 +27568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6872BF-EA12-4909-8C38-56AFC5FB0DC4}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
@@ -26720,6 +28477,76 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95322481-5BBF-4A56-9914-79418416D0F3}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2">
+        <f>B1-1332</f>
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55AC2163-D8C5-47D2-B2CC-21BBFC4B5771}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1">
+        <v>709</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>719</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95B4F40-B183-4124-86C2-CDCC0F988005}">
   <dimension ref="A1:C5"/>

</xml_diff>